<commit_message>
3x and 2x some of the PT slopes
</commit_message>
<xml_diff>
--- a/tools/CMS_Avionics_Channels.xlsx
+++ b/tools/CMS_Avionics_Channels.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Calibration" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="channels" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="calibration" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -114,9 +114,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -188,11 +189,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,8 +216,8 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,7 +251,8 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>100.0093205</v>
+        <f aca="false">100.0093205 * 2</f>
+        <v>200.018641</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0.373452149</v>
@@ -267,7 +269,8 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>100.0120177</v>
+        <f aca="false">100.0120177 * 3</f>
+        <v>300.0360531</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.074545204</v>
@@ -284,7 +287,8 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>499.706495</v>
+        <f aca="false">499.706495 * 3</f>
+        <v>1499.119485</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>-3.510611027</v>
@@ -455,7 +459,7 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
channel config spreadsheet update
</commit_message>
<xml_diff>
--- a/tools/CMS_Avionics_Channels.xlsx
+++ b/tools/CMS_Avionics_Channels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="channels" sheetId="1" state="visible" r:id="rId2"/>
@@ -216,11 +216,11 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.94"/>
@@ -336,7 +336,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>12</v>
@@ -347,7 +347,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>12</v>
@@ -358,7 +358,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>12</v>
@@ -369,7 +369,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>12</v>
@@ -459,11 +459,11 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
added new redline channels to excel doc
</commit_message>
<xml_diff>
--- a/tools/CMS_Avionics_Channels.xlsx
+++ b/tools/CMS_Avionics_Channels.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t xml:space="preserve">OX_LOWER_SETP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FU_UPPER_REDLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FU_LOWER_REDLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OX_UPPER_REDLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OX_LOWER_REDLINE</t>
   </si>
   <si>
     <t xml:space="preserve">FREE_SPACE</t>
@@ -214,13 +226,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.94"/>
@@ -383,11 +395,11 @@
         <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
-        <f aca="false">C3</f>
+        <f aca="false">$C$3</f>
         <v>300.0360531</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">D3</f>
+        <f aca="false">$D$3</f>
         <v>0.074545204</v>
       </c>
       <c r="E11" s="0" t="s">
@@ -402,11 +414,11 @@
         <v>15</v>
       </c>
       <c r="C12" s="0" t="n">
-        <f aca="false">C3</f>
+        <f aca="false">$C$3</f>
         <v>300.0360531</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">D3</f>
+        <f aca="false">$D$3</f>
         <v>0.074545204</v>
       </c>
       <c r="E12" s="0" t="s">
@@ -421,11 +433,11 @@
         <v>16</v>
       </c>
       <c r="C13" s="0" t="n">
-        <f aca="false">C2</f>
+        <f aca="false">$C$2</f>
         <v>300.0279615</v>
       </c>
       <c r="D13" s="0" t="n">
-        <f aca="false">D2</f>
+        <f aca="false">$D$2</f>
         <v>0.373452149</v>
       </c>
       <c r="E13" s="0" t="s">
@@ -440,11 +452,11 @@
         <v>17</v>
       </c>
       <c r="C14" s="0" t="n">
-        <f aca="false">C2</f>
+        <f aca="false">$C$2</f>
         <v>300.0279615</v>
       </c>
       <c r="D14" s="0" t="n">
-        <f aca="false">D2</f>
+        <f aca="false">$D$2</f>
         <v>0.373452149</v>
       </c>
       <c r="E14" s="0" t="s">
@@ -458,19 +470,95 @@
       <c r="B15" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">$C$3</f>
+        <v>300.0360531</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">$D$3</f>
+        <v>0.074545204</v>
+      </c>
       <c r="E15" s="0" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <f aca="false">$C$3</f>
+        <v>300.0360531</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">$D$3</f>
+        <v>0.074545204</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="B17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <f aca="false">$C$2</f>
+        <v>300.0279615</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">$D$2</f>
+        <v>0.373452149</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="0" t="n">
         <v>21</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <f aca="false">$C$2</f>
+        <v>300.0279615</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">$D$2</f>
+        <v>0.373452149</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -495,19 +583,19 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,15 +696,15 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>-143</v>

</xml_diff>

<commit_message>
changed excel channel config to match config.hpp
</commit_message>
<xml_diff>
--- a/tools/CMS_Avionics_Channels.xlsx
+++ b/tools/CMS_Avionics_Channels.xlsx
@@ -229,10 +229,10 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.94"/>
@@ -411,7 +411,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">$C$3</f>
@@ -430,7 +430,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">$C$2</f>
@@ -487,7 +487,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">$C$3</f>
@@ -506,7 +506,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">$C$2</f>
@@ -583,7 +583,7 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>